<commit_message>
changed comments, updated spreadsheets
</commit_message>
<xml_diff>
--- a/results/mismatch_ratio_experiments/plots_eavesdropping.xlsx
+++ b/results/mismatch_ratio_experiments/plots_eavesdropping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlomazzanti/progetti/JuliaProjects/BB84_Protocol/mismatch_ratio_experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlomazzanti/progetti/JuliaProjects/BB84_Protocol/results/mismatch_ratio_experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840EAFAF-3BE9-2B40-8C48-E2842C87F0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF051CC-1DB4-AA48-98AB-92F9521AABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="16900" firstSheet="1" activeTab="4" xr2:uid="{9A08787D-F864-6041-800F-A5D164DD91D4}"/>
+    <workbookView xWindow="220" yWindow="800" windowWidth="29920" windowHeight="16900" firstSheet="1" activeTab="4" xr2:uid="{9A08787D-F864-6041-800F-A5D164DD91D4}"/>
   </bookViews>
   <sheets>
     <sheet name="mismatch_ratios_eavesdropping" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="mismatch_ratios_eavesdroppi (2)" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">'mismatch_ratios_eavesdroppi (2)'!$A$1:$D$12</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">mismatch_ratios_eavesdropping!$A$1:$D$12</definedName>
@@ -4243,6 +4246,386 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="mismatch_ratios_ideal"/>
+      <sheetName val="mismatch_ratios_bitflip"/>
+      <sheetName val="mismatch_ratios_phaseflip"/>
+      <sheetName val="mismatch_ratios_bitphaseflip"/>
+      <sheetName val="Foglio1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>0</v>
+          </cell>
+          <cell r="B2">
+            <v>0.24941663</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>0.1</v>
+          </cell>
+          <cell r="B3">
+            <v>0.25000349999999999</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>0.2</v>
+          </cell>
+          <cell r="B4">
+            <v>0.24960992000000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0.3</v>
+          </cell>
+          <cell r="B5">
+            <v>0.25000655999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>0.4</v>
+          </cell>
+          <cell r="B6">
+            <v>0.24915983</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>0.5</v>
+          </cell>
+          <cell r="B7">
+            <v>0.24823002999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>0.6</v>
+          </cell>
+          <cell r="B8">
+            <v>0.24933675999999999</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>0.7</v>
+          </cell>
+          <cell r="B9">
+            <v>0.25079662000000003</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>0.8</v>
+          </cell>
+          <cell r="B10">
+            <v>0.25107689999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>0.9</v>
+          </cell>
+          <cell r="B11">
+            <v>0.24943989999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+          <cell r="B12">
+            <v>0.25024350000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="A2">
+            <v>0</v>
+          </cell>
+          <cell r="B2">
+            <v>0.24949001000000001</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>0.1</v>
+          </cell>
+          <cell r="B3">
+            <v>0.27475349999999998</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>0.2</v>
+          </cell>
+          <cell r="B4">
+            <v>0.30019699999999999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0.3</v>
+          </cell>
+          <cell r="B5">
+            <v>0.32510339999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>0.4</v>
+          </cell>
+          <cell r="B6">
+            <v>0.35042676</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>0.5</v>
+          </cell>
+          <cell r="B7">
+            <v>0.37506687999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>0.6</v>
+          </cell>
+          <cell r="B8">
+            <v>0.40127993000000001</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>0.7</v>
+          </cell>
+          <cell r="B9">
+            <v>0.42589660000000001</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>0.8</v>
+          </cell>
+          <cell r="B10">
+            <v>0.44993988000000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>0.9</v>
+          </cell>
+          <cell r="B11">
+            <v>0.47563699999999998</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+          <cell r="B12">
+            <v>0.49995336000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="A2">
+            <v>0</v>
+          </cell>
+          <cell r="B2">
+            <v>0.24950673000000001</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>0.1</v>
+          </cell>
+          <cell r="B3">
+            <v>0.27522665000000002</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>0.2</v>
+          </cell>
+          <cell r="B4">
+            <v>0.29773351999999997</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0.3</v>
+          </cell>
+          <cell r="B5">
+            <v>0.32445010000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>0.4</v>
+          </cell>
+          <cell r="B6">
+            <v>0.35152006000000002</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>0.5</v>
+          </cell>
+          <cell r="B7">
+            <v>0.37541667000000001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>0.6</v>
+          </cell>
+          <cell r="B8">
+            <v>0.40148645999999999</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>0.7</v>
+          </cell>
+          <cell r="B9">
+            <v>0.42731646000000001</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>0.8</v>
+          </cell>
+          <cell r="B10">
+            <v>0.45025673999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>0.9</v>
+          </cell>
+          <cell r="B11">
+            <v>0.47581309999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+          <cell r="B12">
+            <v>0.50091339999999995</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="A2">
+            <v>0</v>
+          </cell>
+          <cell r="B2">
+            <v>0.24791326</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>0.1</v>
+          </cell>
+          <cell r="B3">
+            <v>0.30017660000000002</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>0.2</v>
+          </cell>
+          <cell r="B4">
+            <v>0.35213348</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0.3</v>
+          </cell>
+          <cell r="B5">
+            <v>0.39801994000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>0.4</v>
+          </cell>
+          <cell r="B6">
+            <v>0.44839686000000001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>0.5</v>
+          </cell>
+          <cell r="B7">
+            <v>0.49988356</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>0.6</v>
+          </cell>
+          <cell r="B8">
+            <v>0.5502399</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>0.7</v>
+          </cell>
+          <cell r="B9">
+            <v>0.60168034000000004</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>0.8</v>
+          </cell>
+          <cell r="B10">
+            <v>0.65057695000000004</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>0.9</v>
+          </cell>
+          <cell r="B11">
+            <v>0.69885324999999998</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+          <cell r="B12">
+            <v>0.75057019999999997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5426,8 +5809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C090C4CD-E9E9-2F4C-8E92-F13B6983F53F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q63" sqref="Q63"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>